<commit_message>
Added plotting of blanks per blank well.
</commit_message>
<xml_diff>
--- a/plateCoordinates.xlsx
+++ b/plateCoordinates.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="22">
   <si>
     <t>A</t>
   </si>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t>Fill in names of strains/ carbon sources into plate scaffold. Matlab will group data according to names. Do not move scaffold</t>
-  </si>
-  <si>
-    <t>#654wrong=undiluted #654 accidently used</t>
-  </si>
-  <si>
-    <t>contaminated with #553</t>
   </si>
   <si>
     <t>x=not used (don't change name)</t>
@@ -93,11 +87,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00.00.00.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,12 +118,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,25 +148,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -257,6 +250,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -291,6 +285,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,16 +461,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -495,7 +490,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -513,7 +508,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
@@ -555,7 +550,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -599,7 +594,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -632,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>8</v>
@@ -643,7 +638,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -676,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>8</v>
@@ -687,7 +682,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -720,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>8</v>
@@ -731,7 +726,7 @@
       <c r="O7" s="3"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -760,11 +755,11 @@
       <c r="J8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>22</v>
+      <c r="K8" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>8</v>
@@ -775,7 +770,7 @@
       <c r="O8" s="3"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>5</v>
@@ -804,11 +799,11 @@
       <c r="J9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>22</v>
+      <c r="K9" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>8</v>
@@ -819,7 +814,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>6</v>
@@ -848,11 +843,11 @@
       <c r="J10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>8</v>
@@ -863,7 +858,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -892,7 +887,7 @@
       <c r="J11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="9" t="s">
         <v>8</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -907,7 +902,7 @@
       <c r="O11" s="3"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -925,7 +920,7 @@
       <c r="O12" s="3"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -943,7 +938,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -961,9 +956,9 @@
       <c r="O14" s="4"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="8" t="s">
-        <v>19</v>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -981,9 +976,9 @@
       <c r="O15" s="4"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="9" t="s">
-        <v>21</v>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1000,7 +995,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1017,7 +1012,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1033,9 +1028,9 @@
       <c r="O18" s="4"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="8" t="s">
-        <v>23</v>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1053,11 +1048,9 @@
       <c r="O19" s="4"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4"/>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1073,11 +1066,9 @@
       <c r="O20" s="4"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="5"/>
-      <c r="B21" s="4" t="s">
-        <v>18</v>
-      </c>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1093,7 +1084,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1110,7 +1101,7 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1127,7 +1118,7 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1154,24 +1145,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
(cosmetics) updated plateCoordinates example file and added example of how to execute scripts.
</commit_message>
<xml_diff>
--- a/plateCoordinates.xlsx
+++ b/plateCoordinates.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+  <si>
+    <t>Fill in names of strains/ carbon sources into plate scaffold. Matlab will group data according to names. Do not move scaffold</t>
+  </si>
   <si>
     <t>A</t>
   </si>
@@ -39,49 +42,226 @@
     <t>G</t>
   </si>
   <si>
+    <t>blank</t>
+  </si>
+  <si>
     <t>H</t>
   </si>
   <si>
+    <t>x=not used (don't change name)</t>
+  </si>
+  <si>
+    <t>blank= no bacteria (don't change name)</t>
+  </si>
+  <si>
+    <t>further comments:</t>
+  </si>
+  <si>
+    <t>aTc00000s926r2</t>
+  </si>
+  <si>
+    <t>aTc40000s926r2</t>
+  </si>
+  <si>
+    <t>aTc11599s926r2</t>
+  </si>
+  <si>
+    <t>aTc03363s926r2</t>
+  </si>
+  <si>
+    <t>aTc00975s926r2</t>
+  </si>
+  <si>
+    <t>aTc00282s926r2</t>
+  </si>
+  <si>
+    <t>aTc00082s926r2</t>
+  </si>
+  <si>
+    <t>aTc00024s926r2</t>
+  </si>
+  <si>
+    <t>aTc00007s926r2</t>
+  </si>
+  <si>
+    <t>aTc00000s840r2</t>
+  </si>
+  <si>
+    <t>aTc00000s927</t>
+  </si>
+  <si>
+    <t>aTc40000s927</t>
+  </si>
+  <si>
+    <t>aTc11599s927</t>
+  </si>
+  <si>
+    <t>aTc03363s927</t>
+  </si>
+  <si>
+    <t>aTc00975s927</t>
+  </si>
+  <si>
+    <t>aTc00282s927</t>
+  </si>
+  <si>
+    <t>aTc00082s927</t>
+  </si>
+  <si>
+    <t>aTc00024s927</t>
+  </si>
+  <si>
+    <t>aTc00007s927</t>
+  </si>
+  <si>
+    <t>aTc00000s840r3</t>
+  </si>
+  <si>
+    <t>AMP0000s838</t>
+  </si>
+  <si>
+    <t>AMP1000s838</t>
+  </si>
+  <si>
+    <t>AMP0333s838</t>
+  </si>
+  <si>
+    <t>AMP0100s838</t>
+  </si>
+  <si>
+    <t>AMP0033s838</t>
+  </si>
+  <si>
+    <t>AMP0010s838</t>
+  </si>
+  <si>
+    <t>AMP0000s893r1</t>
+  </si>
+  <si>
+    <t>AMP1000s893r1</t>
+  </si>
+  <si>
+    <t>AMP0333s893r1</t>
+  </si>
+  <si>
+    <t>AMP0100s893r1</t>
+  </si>
+  <si>
+    <t>AMP0033s893r1</t>
+  </si>
+  <si>
+    <t>AMP0010s893r1</t>
+  </si>
+  <si>
+    <t>AMP0000s839r1</t>
+  </si>
+  <si>
+    <t>AMP1000s839r1</t>
+  </si>
+  <si>
+    <t>AMP0333s839r1</t>
+  </si>
+  <si>
+    <t>AMP0100s839r1</t>
+  </si>
+  <si>
+    <t>AMP0033s839r1</t>
+  </si>
+  <si>
+    <t>AMP0010s839r1</t>
+  </si>
+  <si>
+    <t>AMP0000s893r2</t>
+  </si>
+  <si>
+    <t>AMP1000s893r2</t>
+  </si>
+  <si>
+    <t>AMP0333s893r2</t>
+  </si>
+  <si>
+    <t>AMP0100s893r2</t>
+  </si>
+  <si>
+    <t>AMP0033s893r2</t>
+  </si>
+  <si>
+    <t>AMP0010s893r2</t>
+  </si>
+  <si>
+    <t>AMP0000s839r2</t>
+  </si>
+  <si>
+    <t>AMP1000s839r2</t>
+  </si>
+  <si>
+    <t>AMP0333s839r2</t>
+  </si>
+  <si>
+    <t>AMP0100s839r2</t>
+  </si>
+  <si>
+    <t>AMP0033s839r2</t>
+  </si>
+  <si>
+    <t>AMP0010s839r2</t>
+  </si>
+  <si>
+    <t>AMP0000s894r1</t>
+  </si>
+  <si>
+    <t>AMP1000s894r1</t>
+  </si>
+  <si>
+    <t>AMP0333s894r1</t>
+  </si>
+  <si>
+    <t>AMP0100s894r1</t>
+  </si>
+  <si>
+    <t>AMP0033s894r1</t>
+  </si>
+  <si>
+    <t>AMP0010s894r1</t>
+  </si>
+  <si>
+    <t>AMP0000s894r2</t>
+  </si>
+  <si>
+    <t>AMP1000s894r2</t>
+  </si>
+  <si>
+    <t>AMP0333s894r2</t>
+  </si>
+  <si>
+    <t>AMP0100s894r2</t>
+  </si>
+  <si>
+    <t>AMP0033s894r2</t>
+  </si>
+  <si>
+    <t>AMP0010s894r2</t>
+  </si>
+  <si>
+    <t>aTc40000blank</t>
+  </si>
+  <si>
+    <t>blankcontam</t>
+  </si>
+  <si>
+    <t>aTc40000s838r2</t>
+  </si>
+  <si>
+    <t>aTc00000s838r2</t>
+  </si>
+  <si>
+    <t>aTc00000s838r3</t>
+  </si>
+  <si>
+    <t>aTc40000s838r3</t>
+  </si>
+  <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>#350</t>
-  </si>
-  <si>
-    <t>#553</t>
-  </si>
-  <si>
-    <t>#636</t>
-  </si>
-  <si>
-    <t>#638</t>
-  </si>
-  <si>
-    <t>#653</t>
-  </si>
-  <si>
-    <t>#654wrong</t>
-  </si>
-  <si>
-    <t>#654</t>
-  </si>
-  <si>
-    <t>Fill in names of strains/ carbon sources into plate scaffold. Matlab will group data according to names. Do not move scaffold</t>
-  </si>
-  <si>
-    <t>x=not used (don't change name)</t>
-  </si>
-  <si>
-    <t>blank</t>
-  </si>
-  <si>
-    <t>blank= no bacteria (don't change name)</t>
-  </si>
-  <si>
-    <t>#350cont</t>
-  </si>
-  <si>
-    <t>further comments:</t>
   </si>
 </sst>
 </file>
@@ -89,23 +269,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="00.00.00.000"/>
+    <numFmt numFmtId="164" formatCode="00.00\.00\.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -117,8 +297,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -134,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,21 +332,83 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFD9D9D9"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -462,17 +704,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.7109375"/>
+    <col min="3" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.7109375"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -553,43 +802,43 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="1"/>
@@ -597,43 +846,43 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="1"/>
@@ -641,43 +890,43 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="1"/>
@@ -685,7 +934,7 @@
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -694,28 +943,28 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>8</v>
@@ -729,43 +978,43 @@
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>20</v>
+        <v>41</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="1"/>
@@ -773,43 +1022,43 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>20</v>
+        <v>53</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="1"/>
@@ -817,43 +1066,43 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>9</v>
+        <v>65</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="1"/>
@@ -861,7 +1110,7 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -873,31 +1122,31 @@
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>8</v>
+        <v>71</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="1"/>
@@ -958,7 +1207,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -978,7 +1227,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1030,7 +1279,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1048,99 +1297,12 @@
       <c r="O19" s="4"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="1"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1148,11 +1310,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.7109375"/>
+  </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -1160,10 +1326,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.7109375"/>
+  </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>